<commit_message>
rorwa 2 casas decimais e calculo de pdd ajustado
</commit_message>
<xml_diff>
--- a/base_indicadores.xlsx
+++ b/base_indicadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fe570407d8e87ac/projetos/simulador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="711" documentId="8_{05C746AA-D6C6-4A60-916E-33F0E5947F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE8A82C5-3F3D-442C-90C3-96AD21F19888}"/>
+  <xr:revisionPtr revIDLastSave="719" documentId="8_{05C746AA-D6C6-4A60-916E-33F0E5947F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B43066A-0F36-44AE-B59A-F27C54D44661}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{26B921F5-7DA8-4D68-B3CE-1C2BB46017C1}"/>
   </bookViews>
@@ -18,11 +18,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicadores!$A$1:$L$169</definedName>
-    <definedName name="_xlcn.WorksheetConnection_indicadoresAL" hidden="1">indicadores!$A:$L</definedName>
+    <definedName name="_xlcn.WorksheetConnection_indicadoresAL1" hidden="1">indicadores!$A:$L</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +65,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Intervalo" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_indicadoresAL"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_indicadoresAL1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -416,10 +416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000%"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,13 +426,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -466,11 +456,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -514,17 +503,13 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -707,7 +692,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{769ACD05-3684-49C7-901B-D3902D254985}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{769ACD05-3684-49C7-901B-D3902D254985}" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -1194,7 +1179,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>101</v>
       </c>
       <c r="B3" t="s">
@@ -1226,7 +1211,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B4">
@@ -1258,7 +1243,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>62</v>
       </c>
       <c r="B5">
@@ -1290,7 +1275,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>100</v>
       </c>
       <c r="B6">
@@ -1322,7 +1307,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B7">
@@ -1354,7 +1339,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B8">
@@ -1386,7 +1371,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B9">
@@ -1418,7 +1403,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>98</v>
       </c>
       <c r="B10">
@@ -1450,7 +1435,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B11">
@@ -1482,7 +1467,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
       <c r="B12">
@@ -1521,9 +1506,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98274D42-0107-497E-BE66-791C82A4E472}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N180"/>
+  <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2720,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
@@ -2731,19 +2718,19 @@
         <v>71</v>
       </c>
       <c r="D32" s="4">
-        <v>477</v>
+        <v>-477</v>
       </c>
       <c r="E32" s="3">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="F32" s="4">
-        <v>327</v>
+        <v>-327</v>
       </c>
       <c r="G32" s="4">
-        <v>641</v>
+        <v>-641</v>
       </c>
       <c r="H32" s="3">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
@@ -2758,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -2769,25 +2756,25 @@
         <v>0</v>
       </c>
       <c r="D33" s="4">
-        <v>3317</v>
+        <v>-3317</v>
       </c>
       <c r="E33" s="3">
-        <v>181</v>
+        <v>-181</v>
       </c>
       <c r="F33" s="4">
-        <v>1585</v>
+        <v>-1585</v>
       </c>
       <c r="G33" s="4">
-        <v>605</v>
+        <v>-605</v>
       </c>
       <c r="H33" s="3">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="I33" s="3">
         <v>0</v>
       </c>
       <c r="J33" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="K33" s="3">
         <v>0</v>
@@ -2796,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
@@ -2807,13 +2794,13 @@
         <v>3</v>
       </c>
       <c r="D34" s="4">
-        <v>2917</v>
+        <v>-2917</v>
       </c>
       <c r="E34" s="3">
-        <v>34</v>
+        <v>-34</v>
       </c>
       <c r="F34" s="4">
-        <v>2269</v>
+        <v>-2269</v>
       </c>
       <c r="G34" s="3">
         <v>0</v>
@@ -2834,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>74</v>
       </c>
@@ -2845,13 +2832,13 @@
         <v>1</v>
       </c>
       <c r="D35" s="4">
-        <v>1957</v>
+        <v>-1957</v>
       </c>
       <c r="E35" s="4">
-        <v>96</v>
+        <v>-96</v>
       </c>
       <c r="F35" s="4">
-        <v>552</v>
+        <v>-552</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -2872,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>74</v>
       </c>
@@ -2883,19 +2870,19 @@
         <v>2</v>
       </c>
       <c r="D36" s="4">
-        <v>68</v>
+        <v>-68</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>208</v>
+        <v>-208</v>
       </c>
       <c r="G36" s="4">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="H36" s="4">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
@@ -2910,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>74</v>
       </c>
@@ -2921,16 +2908,16 @@
         <v>4</v>
       </c>
       <c r="D37" s="4">
-        <v>380</v>
+        <v>-380</v>
       </c>
       <c r="E37" s="3">
-        <v>28</v>
+        <v>-28</v>
       </c>
       <c r="F37" s="4">
-        <v>200</v>
+        <v>-200</v>
       </c>
       <c r="G37" s="4">
-        <v>273</v>
+        <v>-273</v>
       </c>
       <c r="H37" s="4">
         <v>0</v>
@@ -2942,13 +2929,13 @@
         <v>0</v>
       </c>
       <c r="K37" s="4">
-        <v>3891</v>
+        <v>-3891</v>
       </c>
       <c r="L37" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -2959,22 +2946,22 @@
         <v>6</v>
       </c>
       <c r="D38" s="3">
-        <v>-7</v>
+        <v>7</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>210</v>
+        <v>-210</v>
       </c>
       <c r="G38" s="4">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="H38" s="4">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="I38" s="4">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J38" s="3">
         <v>0</v>
@@ -2986,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
@@ -3003,16 +2990,16 @@
         <v>0</v>
       </c>
       <c r="F39" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G39" s="4">
-        <v>1116</v>
+        <v>-1116</v>
       </c>
       <c r="H39" s="4">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="I39" s="4">
-        <v>340</v>
+        <v>-340</v>
       </c>
       <c r="J39" s="3">
         <v>0</v>
@@ -3024,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>74</v>
       </c>
@@ -3035,13 +3022,13 @@
         <v>8</v>
       </c>
       <c r="D40" s="3">
-        <v>29</v>
+        <v>-29</v>
       </c>
       <c r="E40" s="3">
-        <v>213</v>
+        <v>-213</v>
       </c>
       <c r="F40" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
@@ -3062,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
@@ -3079,19 +3066,19 @@
         <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="G41" s="4">
-        <v>41</v>
+        <v>-41</v>
       </c>
       <c r="H41" s="4">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="I41" s="4">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="J41" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K41" s="3">
         <v>0</v>
@@ -3100,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>74</v>
       </c>
@@ -3117,19 +3104,19 @@
         <v>0</v>
       </c>
       <c r="F42" s="3">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="G42" s="4">
-        <v>154</v>
+        <v>-154</v>
       </c>
       <c r="H42" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I42" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J42" s="3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K42" s="3">
         <v>0</v>
@@ -3138,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>74</v>
       </c>
@@ -3158,13 +3145,13 @@
         <v>0</v>
       </c>
       <c r="G43" s="3">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="H43" s="4">
-        <v>21</v>
+        <v>-21</v>
       </c>
       <c r="I43" s="4">
-        <v>897</v>
+        <v>-897</v>
       </c>
       <c r="J43" s="3">
         <v>0</v>
@@ -3177,7 +3164,7 @@
       </c>
       <c r="N43" s="3"/>
     </row>
-    <row r="44" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>74</v>
       </c>
@@ -3200,10 +3187,10 @@
         <v>0</v>
       </c>
       <c r="H44" s="4">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="I44" s="4">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="J44" s="3">
         <v>0</v>
@@ -3216,7 +3203,7 @@
       </c>
       <c r="N44" s="3"/>
     </row>
-    <row r="45" spans="1:14" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>74</v>
       </c>
@@ -3233,19 +3220,19 @@
         <v>0</v>
       </c>
       <c r="F45" s="11">
-        <v>57</v>
+        <v>-57</v>
       </c>
       <c r="G45" s="11">
-        <v>165</v>
+        <v>-165</v>
       </c>
       <c r="H45" s="11">
-        <v>132</v>
+        <v>-132</v>
       </c>
       <c r="I45" s="11">
-        <v>955</v>
+        <v>-955</v>
       </c>
       <c r="J45" s="10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K45" s="11">
         <v>0</v>
@@ -7245,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
         <v>62</v>
       </c>
@@ -7283,7 +7270,7 @@
         <v>81922</v>
       </c>
     </row>
-    <row r="152" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="9" t="s">
         <v>62</v>
       </c>
@@ -7321,7 +7308,7 @@
         <v>-26529</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>62</v>
       </c>
@@ -7359,7 +7346,7 @@
         <v>55393</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>62</v>
       </c>
@@ -7397,7 +7384,7 @@
         <v>-3107</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>62</v>
       </c>
@@ -7435,7 +7422,7 @@
         <v>-314</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>62</v>
       </c>
@@ -7473,7 +7460,7 @@
         <v>-26129</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>62</v>
       </c>
@@ -7511,7 +7498,7 @@
         <v>25843</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>62</v>
       </c>
@@ -7549,7 +7536,7 @@
         <v>-10607</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>62</v>
       </c>
@@ -7587,7 +7574,7 @@
         <v>15236</v>
       </c>
     </row>
-    <row r="160" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>62</v>
       </c>
@@ -7978,14 +7965,11 @@
       <c r="K171" s="6"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E180" s="15"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:L169" xr:uid="{98274D42-0107-497E-BE66-791C82A4E472}">
     <filterColumn colId="1">
       <filters>
-        <filter val="cascada"/>
+        <filter val="provisao"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>